<commit_message>
add df of seriea/ligue1 with odds
</commit_message>
<xml_diff>
--- a/FantaSoccer/MyModule/Test_MultiMetodo_Ligue1_with_odds.xlsx
+++ b/FantaSoccer/MyModule/Test_MultiMetodo_Ligue1_with_odds.xlsx
@@ -792,8 +792,23 @@
       <c r="Q4">
         <v>0</v>
       </c>
+      <c r="R4">
+        <v>-1</v>
+      </c>
+      <c r="S4">
+        <v>2.15</v>
+      </c>
+      <c r="T4">
+        <v>3.5</v>
+      </c>
+      <c r="U4">
+        <v>3.2</v>
+      </c>
       <c r="V4">
-        <v>0</v>
+        <v>3.2</v>
+      </c>
+      <c r="W4">
+        <v>3.5</v>
       </c>
       <c r="X4">
         <v>0</v>
@@ -802,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="Z4">
-        <v>0</v>
+        <v>2.285714285714286</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -854,8 +869,23 @@
       <c r="Q5">
         <v>1</v>
       </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>1.06</v>
+      </c>
+      <c r="T5">
+        <v>12</v>
+      </c>
+      <c r="U5">
+        <v>23</v>
+      </c>
       <c r="V5">
-        <v>0</v>
+        <v>1.06</v>
+      </c>
+      <c r="W5">
+        <v>1.06</v>
       </c>
       <c r="X5">
         <v>0</v>
@@ -864,7 +894,7 @@
         <v>0</v>
       </c>
       <c r="Z5">
-        <v>0</v>
+        <v>0.9716666666666667</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -996,14 +1026,32 @@
       <c r="Q7">
         <v>1</v>
       </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>3.5</v>
+      </c>
+      <c r="T7">
+        <v>3.1</v>
+      </c>
+      <c r="U7">
+        <v>2.2</v>
+      </c>
       <c r="V7">
-        <v>0</v>
+        <v>3.1</v>
+      </c>
+      <c r="W7">
+        <v>3.1</v>
+      </c>
+      <c r="X7">
+        <v>3.1</v>
       </c>
       <c r="Y7">
         <v>0</v>
       </c>
       <c r="Z7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -1055,8 +1103,23 @@
       <c r="Q8">
         <v>0</v>
       </c>
+      <c r="R8">
+        <v>-1</v>
+      </c>
+      <c r="S8">
+        <v>2.87</v>
+      </c>
+      <c r="T8">
+        <v>3.4</v>
+      </c>
+      <c r="U8">
+        <v>2.4</v>
+      </c>
       <c r="V8">
-        <v>0</v>
+        <v>2.4</v>
+      </c>
+      <c r="W8">
+        <v>3.4</v>
       </c>
       <c r="X8">
         <v>0</v>
@@ -1065,7 +1128,7 @@
         <v>0</v>
       </c>
       <c r="Z8">
-        <v>0</v>
+        <v>1.694117647058824</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -1117,8 +1180,23 @@
       <c r="Q9">
         <v>1</v>
       </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>1.65</v>
+      </c>
+      <c r="T9">
+        <v>4</v>
+      </c>
+      <c r="U9">
+        <v>4.75</v>
+      </c>
       <c r="V9">
-        <v>0</v>
+        <v>1.65</v>
+      </c>
+      <c r="W9">
+        <v>1.65</v>
       </c>
       <c r="X9">
         <v>0</v>
@@ -1127,7 +1205,7 @@
         <v>0</v>
       </c>
       <c r="Z9">
-        <v>0</v>
+        <v>1.2375</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -1179,8 +1257,23 @@
       <c r="Q10">
         <v>1</v>
       </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>2.37</v>
+      </c>
+      <c r="T10">
+        <v>3.2</v>
+      </c>
+      <c r="U10">
+        <v>3.1</v>
+      </c>
       <c r="V10">
-        <v>0</v>
+        <v>2.37</v>
+      </c>
+      <c r="W10">
+        <v>2.37</v>
       </c>
       <c r="X10">
         <v>0</v>
@@ -1189,7 +1282,7 @@
         <v>0</v>
       </c>
       <c r="Z10">
-        <v>0</v>
+        <v>1.629375</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -1552,8 +1645,23 @@
       <c r="Q15">
         <v>0</v>
       </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>1.75</v>
+      </c>
+      <c r="T15">
+        <v>3.6</v>
+      </c>
+      <c r="U15">
+        <v>4.75</v>
+      </c>
       <c r="V15">
-        <v>0</v>
+        <v>3.6</v>
+      </c>
+      <c r="W15">
+        <v>1.75</v>
       </c>
       <c r="X15">
         <v>0</v>
@@ -1562,7 +1670,7 @@
         <v>0</v>
       </c>
       <c r="Z15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:26">
@@ -1768,8 +1876,23 @@
       <c r="Q18">
         <v>1</v>
       </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <v>1.4</v>
+      </c>
+      <c r="T18">
+        <v>4.75</v>
+      </c>
+      <c r="U18">
+        <v>7.5</v>
+      </c>
       <c r="V18">
-        <v>0</v>
+        <v>1.4</v>
+      </c>
+      <c r="W18">
+        <v>1.4</v>
       </c>
       <c r="X18">
         <v>0</v>
@@ -1778,7 +1901,7 @@
         <v>0</v>
       </c>
       <c r="Z18">
-        <v>0</v>
+        <v>1.105263157894737</v>
       </c>
     </row>
     <row r="19" spans="1:26">
@@ -1833,11 +1956,32 @@
       <c r="Q19">
         <v>1</v>
       </c>
+      <c r="R19">
+        <v>-1</v>
+      </c>
+      <c r="S19">
+        <v>2.87</v>
+      </c>
+      <c r="T19">
+        <v>3.3</v>
+      </c>
+      <c r="U19">
+        <v>2.45</v>
+      </c>
       <c r="V19">
-        <v>0</v>
+        <v>2.45</v>
+      </c>
+      <c r="W19">
+        <v>2.45</v>
+      </c>
+      <c r="X19">
+        <v>3.3</v>
+      </c>
+      <c r="Y19">
+        <v>1.406086956521739</v>
       </c>
       <c r="Z19">
-        <v>0</v>
+        <v>1.707575757575758</v>
       </c>
     </row>
     <row r="20" spans="1:26">
@@ -1889,8 +2033,23 @@
       <c r="Q20">
         <v>0</v>
       </c>
+      <c r="R20">
+        <v>-1</v>
+      </c>
+      <c r="S20">
+        <v>3.2</v>
+      </c>
+      <c r="T20">
+        <v>3.6</v>
+      </c>
+      <c r="U20">
+        <v>2.15</v>
+      </c>
       <c r="V20">
-        <v>0</v>
+        <v>2.15</v>
+      </c>
+      <c r="W20">
+        <v>3.2</v>
       </c>
       <c r="X20">
         <v>0</v>
@@ -1899,7 +2058,7 @@
         <v>0</v>
       </c>
       <c r="Z20">
-        <v>0</v>
+        <v>1.552777777777778</v>
       </c>
     </row>
     <row r="21" spans="1:26">
@@ -1954,11 +2113,32 @@
       <c r="Q21">
         <v>0</v>
       </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>1.4</v>
+      </c>
+      <c r="T21">
+        <v>5.25</v>
+      </c>
+      <c r="U21">
+        <v>6.5</v>
+      </c>
       <c r="V21">
-        <v>0</v>
+        <v>1.4</v>
+      </c>
+      <c r="W21">
+        <v>5.25</v>
+      </c>
+      <c r="X21">
+        <v>1.4</v>
+      </c>
+      <c r="Y21">
+        <v>1.105263157894737</v>
       </c>
       <c r="Z21">
-        <v>0</v>
+        <v>1.133333333333333</v>
       </c>
     </row>
     <row r="22" spans="1:26">
@@ -2010,8 +2190,23 @@
       <c r="Q22">
         <v>0</v>
       </c>
+      <c r="R22">
+        <v>-1</v>
+      </c>
+      <c r="S22">
+        <v>5</v>
+      </c>
+      <c r="T22">
+        <v>4.2</v>
+      </c>
+      <c r="U22">
+        <v>1.61</v>
+      </c>
       <c r="V22">
-        <v>0</v>
+        <v>1.61</v>
+      </c>
+      <c r="W22">
+        <v>4.2</v>
       </c>
       <c r="X22">
         <v>0</v>
@@ -2020,7 +2215,7 @@
         <v>0</v>
       </c>
       <c r="Z22">
-        <v>0</v>
+        <v>1.226666666666667</v>
       </c>
     </row>
     <row r="23" spans="1:26">
@@ -2149,8 +2344,23 @@
       <c r="Q24">
         <v>1</v>
       </c>
+      <c r="R24">
+        <v>1</v>
+      </c>
+      <c r="S24">
+        <v>2.1</v>
+      </c>
+      <c r="T24">
+        <v>3.5</v>
+      </c>
+      <c r="U24">
+        <v>3.4</v>
+      </c>
       <c r="V24">
-        <v>0</v>
+        <v>2.1</v>
+      </c>
+      <c r="W24">
+        <v>2.1</v>
       </c>
       <c r="X24">
         <v>0</v>
@@ -2159,7 +2369,7 @@
         <v>0</v>
       </c>
       <c r="Z24">
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="25" spans="1:26">
@@ -2211,8 +2421,23 @@
       <c r="Q25">
         <v>0</v>
       </c>
+      <c r="R25">
+        <v>-1</v>
+      </c>
+      <c r="S25">
+        <v>3.5</v>
+      </c>
+      <c r="T25">
+        <v>3.4</v>
+      </c>
+      <c r="U25">
+        <v>2.15</v>
+      </c>
       <c r="V25">
-        <v>0</v>
+        <v>2.15</v>
+      </c>
+      <c r="W25">
+        <v>3.4</v>
       </c>
       <c r="X25">
         <v>0</v>
@@ -2221,7 +2446,7 @@
         <v>0</v>
       </c>
       <c r="Z25">
-        <v>0</v>
+        <v>1.517647058823529</v>
       </c>
     </row>
     <row r="26" spans="1:26">
@@ -2492,8 +2717,23 @@
       <c r="Q29">
         <v>0</v>
       </c>
+      <c r="R29">
+        <v>1</v>
+      </c>
+      <c r="S29">
+        <v>5.25</v>
+      </c>
+      <c r="T29">
+        <v>4.75</v>
+      </c>
+      <c r="U29">
+        <v>1.5</v>
+      </c>
       <c r="V29">
-        <v>0</v>
+        <v>5.25</v>
+      </c>
+      <c r="W29">
+        <v>1.5</v>
       </c>
       <c r="X29">
         <v>0</v>
@@ -2502,7 +2742,7 @@
         <v>0</v>
       </c>
       <c r="Z29">
-        <v>0</v>
+        <v>4.144736842105263</v>
       </c>
     </row>
     <row r="30" spans="1:26">
@@ -2554,8 +2794,23 @@
       <c r="Q30">
         <v>0</v>
       </c>
+      <c r="R30">
+        <v>1</v>
+      </c>
+      <c r="S30">
+        <v>2.05</v>
+      </c>
+      <c r="T30">
+        <v>3.5</v>
+      </c>
+      <c r="U30">
+        <v>3.6</v>
+      </c>
       <c r="V30">
-        <v>0</v>
+        <v>2.05</v>
+      </c>
+      <c r="W30">
+        <v>3.5</v>
       </c>
       <c r="X30">
         <v>0</v>
@@ -2564,7 +2819,7 @@
         <v>0</v>
       </c>
       <c r="Z30">
-        <v>0</v>
+        <v>1.464285714285714</v>
       </c>
     </row>
     <row r="31" spans="1:26">
@@ -2770,8 +3025,23 @@
       <c r="Q33">
         <v>0</v>
       </c>
+      <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <v>1.12</v>
+      </c>
+      <c r="T33">
+        <v>8.5</v>
+      </c>
+      <c r="U33">
+        <v>17</v>
+      </c>
       <c r="V33">
-        <v>0</v>
+        <v>8.5</v>
+      </c>
+      <c r="W33">
+        <v>1.12</v>
       </c>
       <c r="X33">
         <v>0</v>
@@ -2780,7 +3050,7 @@
         <v>0</v>
       </c>
       <c r="Z33">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:26">
@@ -2909,8 +3179,23 @@
       <c r="Q35">
         <v>0</v>
       </c>
+      <c r="R35">
+        <v>-1</v>
+      </c>
+      <c r="S35">
+        <v>1.75</v>
+      </c>
+      <c r="T35">
+        <v>3.6</v>
+      </c>
+      <c r="U35">
+        <v>4.5</v>
+      </c>
       <c r="V35">
-        <v>0</v>
+        <v>4.5</v>
+      </c>
+      <c r="W35">
+        <v>1.75</v>
       </c>
       <c r="X35">
         <v>0</v>
@@ -2919,7 +3204,7 @@
         <v>0</v>
       </c>
       <c r="Z35">
-        <v>0</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="36" spans="1:26">
@@ -2971,8 +3256,23 @@
       <c r="Q36">
         <v>0</v>
       </c>
+      <c r="R36">
+        <v>0</v>
+      </c>
+      <c r="S36">
+        <v>4.75</v>
+      </c>
+      <c r="T36">
+        <v>3.6</v>
+      </c>
+      <c r="U36">
+        <v>1.72</v>
+      </c>
       <c r="V36">
-        <v>0</v>
+        <v>3.6</v>
+      </c>
+      <c r="W36">
+        <v>1.72</v>
       </c>
       <c r="X36">
         <v>0</v>
@@ -2981,7 +3281,7 @@
         <v>0</v>
       </c>
       <c r="Z36">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:26">
@@ -3110,8 +3410,23 @@
       <c r="Q38">
         <v>1</v>
       </c>
+      <c r="R38">
+        <v>1</v>
+      </c>
+      <c r="S38">
+        <v>1.4</v>
+      </c>
+      <c r="T38">
+        <v>4.75</v>
+      </c>
+      <c r="U38">
+        <v>7</v>
+      </c>
       <c r="V38">
-        <v>0</v>
+        <v>1.4</v>
+      </c>
+      <c r="W38">
+        <v>1.4</v>
       </c>
       <c r="X38">
         <v>0</v>
@@ -3120,7 +3435,7 @@
         <v>0</v>
       </c>
       <c r="Z38">
-        <v>0</v>
+        <v>1.105263157894737</v>
       </c>
     </row>
     <row r="39" spans="1:26">
@@ -3172,8 +3487,23 @@
       <c r="Q39">
         <v>0</v>
       </c>
+      <c r="R39">
+        <v>1</v>
+      </c>
+      <c r="S39">
+        <v>2.05</v>
+      </c>
+      <c r="T39">
+        <v>3.4</v>
+      </c>
+      <c r="U39">
+        <v>3.5</v>
+      </c>
       <c r="V39">
-        <v>0</v>
+        <v>2.05</v>
+      </c>
+      <c r="W39">
+        <v>3.4</v>
       </c>
       <c r="X39">
         <v>0</v>
@@ -3182,7 +3512,7 @@
         <v>0</v>
       </c>
       <c r="Z39">
-        <v>0</v>
+        <v>1.447058823529412</v>
       </c>
     </row>
     <row r="40" spans="1:26">
@@ -3311,8 +3641,23 @@
       <c r="Q41">
         <v>1</v>
       </c>
+      <c r="R41">
+        <v>0</v>
+      </c>
+      <c r="S41">
+        <v>3.2</v>
+      </c>
+      <c r="T41">
+        <v>3.2</v>
+      </c>
+      <c r="U41">
+        <v>2.3</v>
+      </c>
       <c r="V41">
-        <v>0</v>
+        <v>3.2</v>
+      </c>
+      <c r="W41">
+        <v>3.2</v>
       </c>
       <c r="X41">
         <v>0</v>
@@ -3321,7 +3666,7 @@
         <v>0</v>
       </c>
       <c r="Z41">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:26">
@@ -3527,8 +3872,23 @@
       <c r="Q44">
         <v>0</v>
       </c>
+      <c r="R44">
+        <v>0</v>
+      </c>
+      <c r="S44">
+        <v>3</v>
+      </c>
+      <c r="T44">
+        <v>3.4</v>
+      </c>
+      <c r="U44">
+        <v>2.37</v>
+      </c>
       <c r="V44">
-        <v>0</v>
+        <v>3.4</v>
+      </c>
+      <c r="W44">
+        <v>3</v>
       </c>
       <c r="X44">
         <v>0</v>
@@ -3537,7 +3897,7 @@
         <v>0</v>
       </c>
       <c r="Z44">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:26">
@@ -3749,8 +4109,23 @@
       <c r="Q47">
         <v>1</v>
       </c>
+      <c r="R47">
+        <v>-1</v>
+      </c>
+      <c r="S47">
+        <v>5.75</v>
+      </c>
+      <c r="T47">
+        <v>4.33</v>
+      </c>
+      <c r="U47">
+        <v>1.55</v>
+      </c>
       <c r="V47">
-        <v>0</v>
+        <v>1.55</v>
+      </c>
+      <c r="W47">
+        <v>1.55</v>
       </c>
       <c r="X47">
         <v>0</v>
@@ -3759,7 +4134,7 @@
         <v>0</v>
       </c>
       <c r="Z47">
-        <v>0</v>
+        <v>1.19203233256351</v>
       </c>
     </row>
     <row r="48" spans="1:26">
@@ -3811,8 +4186,23 @@
       <c r="Q48">
         <v>1</v>
       </c>
+      <c r="R48">
+        <v>-1</v>
+      </c>
+      <c r="S48">
+        <v>5.25</v>
+      </c>
+      <c r="T48">
+        <v>3.8</v>
+      </c>
+      <c r="U48">
+        <v>1.66</v>
+      </c>
       <c r="V48">
-        <v>0</v>
+        <v>1.66</v>
+      </c>
+      <c r="W48">
+        <v>1.66</v>
       </c>
       <c r="X48">
         <v>0</v>
@@ -3821,7 +4211,7 @@
         <v>0</v>
       </c>
       <c r="Z48">
-        <v>0</v>
+        <v>1.223157894736842</v>
       </c>
     </row>
     <row r="49" spans="1:26">
@@ -3873,8 +4263,23 @@
       <c r="Q49">
         <v>1</v>
       </c>
+      <c r="R49">
+        <v>-1</v>
+      </c>
+      <c r="S49">
+        <v>6.5</v>
+      </c>
+      <c r="T49">
+        <v>4.75</v>
+      </c>
+      <c r="U49">
+        <v>1.44</v>
+      </c>
       <c r="V49">
-        <v>0</v>
+        <v>1.44</v>
+      </c>
+      <c r="W49">
+        <v>1.44</v>
       </c>
       <c r="X49">
         <v>0</v>
@@ -3883,7 +4288,7 @@
         <v>0</v>
       </c>
       <c r="Z49">
-        <v>0</v>
+        <v>1.136842105263158</v>
       </c>
     </row>
     <row r="50" spans="1:26">
@@ -3935,8 +4340,23 @@
       <c r="Q50">
         <v>0</v>
       </c>
+      <c r="R50">
+        <v>-1</v>
+      </c>
+      <c r="S50">
+        <v>2.15</v>
+      </c>
+      <c r="T50">
+        <v>3.3</v>
+      </c>
+      <c r="U50">
+        <v>3.5</v>
+      </c>
       <c r="V50">
-        <v>0</v>
+        <v>3.5</v>
+      </c>
+      <c r="W50">
+        <v>3.3</v>
       </c>
       <c r="X50">
         <v>0</v>
@@ -3945,7 +4365,7 @@
         <v>0</v>
       </c>
       <c r="Z50">
-        <v>0</v>
+        <v>2.439393939393939</v>
       </c>
     </row>
     <row r="51" spans="1:26">
@@ -3997,8 +4417,23 @@
       <c r="Q51">
         <v>1</v>
       </c>
+      <c r="R51">
+        <v>0</v>
+      </c>
+      <c r="S51">
+        <v>2.5</v>
+      </c>
+      <c r="T51">
+        <v>3.4</v>
+      </c>
+      <c r="U51">
+        <v>2.8</v>
+      </c>
       <c r="V51">
-        <v>0</v>
+        <v>3.4</v>
+      </c>
+      <c r="W51">
+        <v>3.4</v>
       </c>
       <c r="X51">
         <v>0</v>
@@ -4007,7 +4442,7 @@
         <v>0</v>
       </c>
       <c r="Z51">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:26">
@@ -4059,8 +4494,23 @@
       <c r="Q52">
         <v>0</v>
       </c>
+      <c r="R52">
+        <v>0</v>
+      </c>
+      <c r="S52">
+        <v>2.37</v>
+      </c>
+      <c r="T52">
+        <v>3.4</v>
+      </c>
+      <c r="U52">
+        <v>2.9</v>
+      </c>
       <c r="V52">
-        <v>0</v>
+        <v>3.4</v>
+      </c>
+      <c r="W52">
+        <v>2.9</v>
       </c>
       <c r="X52">
         <v>0</v>
@@ -4069,7 +4519,7 @@
         <v>0</v>
       </c>
       <c r="Z52">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:26">
@@ -4275,8 +4725,23 @@
       <c r="Q55">
         <v>1</v>
       </c>
+      <c r="R55">
+        <v>0</v>
+      </c>
+      <c r="S55">
+        <v>1.72</v>
+      </c>
+      <c r="T55">
+        <v>3.75</v>
+      </c>
+      <c r="U55">
+        <v>4.5</v>
+      </c>
       <c r="V55">
-        <v>0</v>
+        <v>3.75</v>
+      </c>
+      <c r="W55">
+        <v>3.75</v>
       </c>
       <c r="X55">
         <v>0</v>
@@ -4285,7 +4750,7 @@
         <v>0</v>
       </c>
       <c r="Z55">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:26">
@@ -4494,8 +4959,23 @@
       <c r="Q58">
         <v>0</v>
       </c>
+      <c r="R58">
+        <v>-1</v>
+      </c>
+      <c r="S58">
+        <v>1.57</v>
+      </c>
+      <c r="T58">
+        <v>4.75</v>
+      </c>
+      <c r="U58">
+        <v>4.5</v>
+      </c>
       <c r="V58">
-        <v>0</v>
+        <v>4.5</v>
+      </c>
+      <c r="W58">
+        <v>4.75</v>
       </c>
       <c r="X58">
         <v>0</v>
@@ -4504,7 +4984,7 @@
         <v>0</v>
       </c>
       <c r="Z58">
-        <v>0</v>
+        <v>3.552631578947369</v>
       </c>
     </row>
     <row r="59" spans="1:26">
@@ -4556,8 +5036,23 @@
       <c r="Q59">
         <v>0</v>
       </c>
+      <c r="R59">
+        <v>1</v>
+      </c>
+      <c r="S59">
+        <v>2.75</v>
+      </c>
+      <c r="T59">
+        <v>3.5</v>
+      </c>
+      <c r="U59">
+        <v>2.4</v>
+      </c>
       <c r="V59">
-        <v>0</v>
+        <v>2.75</v>
+      </c>
+      <c r="W59">
+        <v>3.5</v>
       </c>
       <c r="X59">
         <v>0</v>
@@ -4566,7 +5061,7 @@
         <v>0</v>
       </c>
       <c r="Z59">
-        <v>0</v>
+        <v>1.964285714285714</v>
       </c>
     </row>
     <row r="60" spans="1:26">
@@ -4618,8 +5113,23 @@
       <c r="Q60">
         <v>1</v>
       </c>
+      <c r="R60">
+        <v>0</v>
+      </c>
+      <c r="S60">
+        <v>2</v>
+      </c>
+      <c r="T60">
+        <v>3.25</v>
+      </c>
+      <c r="U60">
+        <v>3.9</v>
+      </c>
       <c r="V60">
-        <v>0</v>
+        <v>3.25</v>
+      </c>
+      <c r="W60">
+        <v>3.25</v>
       </c>
       <c r="X60">
         <v>0</v>
@@ -4628,7 +5138,7 @@
         <v>0</v>
       </c>
       <c r="Z60">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:26">
@@ -4680,8 +5190,23 @@
       <c r="Q61">
         <v>0</v>
       </c>
+      <c r="R61">
+        <v>-1</v>
+      </c>
+      <c r="S61">
+        <v>2.9</v>
+      </c>
+      <c r="T61">
+        <v>3.3</v>
+      </c>
+      <c r="U61">
+        <v>2.37</v>
+      </c>
       <c r="V61">
-        <v>0</v>
+        <v>2.37</v>
+      </c>
+      <c r="W61">
+        <v>3.3</v>
       </c>
       <c r="X61">
         <v>0</v>
@@ -4690,7 +5215,7 @@
         <v>0</v>
       </c>
       <c r="Z61">
-        <v>0</v>
+        <v>1.651818181818182</v>
       </c>
     </row>
     <row r="62" spans="1:26">
@@ -4742,8 +5267,23 @@
       <c r="Q62">
         <v>0</v>
       </c>
+      <c r="R62">
+        <v>-1</v>
+      </c>
+      <c r="S62">
+        <v>2.15</v>
+      </c>
+      <c r="T62">
+        <v>3.5</v>
+      </c>
+      <c r="U62">
+        <v>3.3</v>
+      </c>
       <c r="V62">
-        <v>0</v>
+        <v>3.3</v>
+      </c>
+      <c r="W62">
+        <v>3.5</v>
       </c>
       <c r="X62">
         <v>0</v>
@@ -4752,7 +5292,7 @@
         <v>0</v>
       </c>
       <c r="Z62">
-        <v>0</v>
+        <v>2.357142857142857</v>
       </c>
     </row>
     <row r="63" spans="1:26">
@@ -4804,8 +5344,23 @@
       <c r="Q63">
         <v>0</v>
       </c>
+      <c r="R63">
+        <v>-1</v>
+      </c>
+      <c r="S63">
+        <v>2.15</v>
+      </c>
+      <c r="T63">
+        <v>3.4</v>
+      </c>
+      <c r="U63">
+        <v>3.4</v>
+      </c>
       <c r="V63">
-        <v>0</v>
+        <v>3.4</v>
+      </c>
+      <c r="W63">
+        <v>2.15</v>
       </c>
       <c r="X63">
         <v>0</v>
@@ -4814,7 +5369,7 @@
         <v>0</v>
       </c>
       <c r="Z63">
-        <v>0</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="64" spans="1:26">
@@ -4869,11 +5424,32 @@
       <c r="Q64">
         <v>1</v>
       </c>
+      <c r="R64">
+        <v>0</v>
+      </c>
+      <c r="S64">
+        <v>1.33</v>
+      </c>
+      <c r="T64">
+        <v>5.25</v>
+      </c>
+      <c r="U64">
+        <v>9</v>
+      </c>
       <c r="V64">
-        <v>0</v>
+        <v>5.25</v>
+      </c>
+      <c r="W64">
+        <v>5.25</v>
+      </c>
+      <c r="X64">
+        <v>1.33</v>
+      </c>
+      <c r="Y64">
+        <v>1.061170212765957</v>
       </c>
       <c r="Z64">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:26">
@@ -4925,8 +5501,23 @@
       <c r="Q65">
         <v>1</v>
       </c>
+      <c r="R65">
+        <v>-1</v>
+      </c>
+      <c r="S65">
+        <v>6.5</v>
+      </c>
+      <c r="T65">
+        <v>4.33</v>
+      </c>
+      <c r="U65">
+        <v>1.5</v>
+      </c>
       <c r="V65">
-        <v>0</v>
+        <v>1.5</v>
+      </c>
+      <c r="W65">
+        <v>1.5</v>
       </c>
       <c r="X65">
         <v>0</v>
@@ -4935,7 +5526,7 @@
         <v>0</v>
       </c>
       <c r="Z65">
-        <v>0</v>
+        <v>1.153579676674365</v>
       </c>
     </row>
     <row r="66" spans="1:26">
@@ -5064,8 +5655,23 @@
       <c r="Q67">
         <v>1</v>
       </c>
+      <c r="R67">
+        <v>1</v>
+      </c>
+      <c r="S67">
+        <v>1.12</v>
+      </c>
+      <c r="T67">
+        <v>9</v>
+      </c>
+      <c r="U67">
+        <v>19</v>
+      </c>
       <c r="V67">
-        <v>0</v>
+        <v>1.12</v>
+      </c>
+      <c r="W67">
+        <v>1.12</v>
       </c>
       <c r="X67">
         <v>0</v>
@@ -5074,7 +5680,7 @@
         <v>0</v>
       </c>
       <c r="Z67">
-        <v>0</v>
+        <v>0.9955555555555556</v>
       </c>
     </row>
     <row r="68" spans="1:26">
@@ -5126,8 +5732,23 @@
       <c r="Q68">
         <v>0</v>
       </c>
+      <c r="R68">
+        <v>1</v>
+      </c>
+      <c r="S68">
+        <v>2.4</v>
+      </c>
+      <c r="T68">
+        <v>3.4</v>
+      </c>
+      <c r="U68">
+        <v>2.87</v>
+      </c>
       <c r="V68">
-        <v>0</v>
+        <v>2.4</v>
+      </c>
+      <c r="W68">
+        <v>2.87</v>
       </c>
       <c r="X68">
         <v>0</v>
@@ -5136,7 +5757,7 @@
         <v>0</v>
       </c>
       <c r="Z68">
-        <v>0</v>
+        <v>1.694117647058824</v>
       </c>
     </row>
     <row r="69" spans="1:26">
@@ -5345,11 +5966,32 @@
       <c r="Q71">
         <v>1</v>
       </c>
+      <c r="R71">
+        <v>-1</v>
+      </c>
+      <c r="S71">
+        <v>3.4</v>
+      </c>
+      <c r="T71">
+        <v>3.5</v>
+      </c>
+      <c r="U71">
+        <v>2.1</v>
+      </c>
       <c r="V71">
-        <v>0</v>
+        <v>2.1</v>
+      </c>
+      <c r="W71">
+        <v>2.1</v>
+      </c>
+      <c r="X71">
+        <v>3.5</v>
+      </c>
+      <c r="Y71">
+        <v>1.3125</v>
       </c>
       <c r="Z71">
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="72" spans="1:26">
@@ -5478,8 +6120,23 @@
       <c r="Q73">
         <v>0</v>
       </c>
+      <c r="R73">
+        <v>-1</v>
+      </c>
+      <c r="S73">
+        <v>2.2</v>
+      </c>
+      <c r="T73">
+        <v>3.3</v>
+      </c>
+      <c r="U73">
+        <v>3.25</v>
+      </c>
       <c r="V73">
-        <v>0</v>
+        <v>3.25</v>
+      </c>
+      <c r="W73">
+        <v>3.3</v>
       </c>
       <c r="X73">
         <v>0</v>
@@ -5488,7 +6145,7 @@
         <v>0</v>
       </c>
       <c r="Z73">
-        <v>0</v>
+        <v>2.265151515151515</v>
       </c>
     </row>
     <row r="74" spans="1:26">
@@ -5617,8 +6274,23 @@
       <c r="Q75">
         <v>0</v>
       </c>
+      <c r="R75">
+        <v>-1</v>
+      </c>
+      <c r="S75">
+        <v>6.5</v>
+      </c>
+      <c r="T75">
+        <v>4.33</v>
+      </c>
+      <c r="U75">
+        <v>1.5</v>
+      </c>
       <c r="V75">
-        <v>0</v>
+        <v>1.5</v>
+      </c>
+      <c r="W75">
+        <v>4.33</v>
       </c>
       <c r="X75">
         <v>0</v>
@@ -5627,7 +6299,7 @@
         <v>0</v>
       </c>
       <c r="Z75">
-        <v>0</v>
+        <v>1.153579676674365</v>
       </c>
     </row>
     <row r="76" spans="1:26">
@@ -5759,8 +6431,23 @@
       <c r="Q77">
         <v>1</v>
       </c>
+      <c r="R77">
+        <v>0</v>
+      </c>
+      <c r="S77">
+        <v>4</v>
+      </c>
+      <c r="T77">
+        <v>3.8</v>
+      </c>
+      <c r="U77">
+        <v>1.85</v>
+      </c>
       <c r="V77">
-        <v>0</v>
+        <v>3.8</v>
+      </c>
+      <c r="W77">
+        <v>3.8</v>
       </c>
       <c r="X77">
         <v>0</v>
@@ -5769,7 +6456,7 @@
         <v>0</v>
       </c>
       <c r="Z77">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:26">
@@ -5898,8 +6585,23 @@
       <c r="Q79">
         <v>1</v>
       </c>
+      <c r="R79">
+        <v>-1</v>
+      </c>
+      <c r="S79">
+        <v>6.5</v>
+      </c>
+      <c r="T79">
+        <v>4</v>
+      </c>
+      <c r="U79">
+        <v>1.55</v>
+      </c>
       <c r="V79">
-        <v>0</v>
+        <v>1.55</v>
+      </c>
+      <c r="W79">
+        <v>1.55</v>
       </c>
       <c r="X79">
         <v>0</v>
@@ -5908,7 +6610,7 @@
         <v>0</v>
       </c>
       <c r="Z79">
-        <v>0</v>
+        <v>1.1625</v>
       </c>
     </row>
     <row r="80" spans="1:26">
@@ -5960,8 +6662,23 @@
       <c r="Q80">
         <v>0</v>
       </c>
+      <c r="R80">
+        <v>0</v>
+      </c>
+      <c r="S80">
+        <v>1.75</v>
+      </c>
+      <c r="T80">
+        <v>3.6</v>
+      </c>
+      <c r="U80">
+        <v>5</v>
+      </c>
       <c r="V80">
-        <v>0</v>
+        <v>3.6</v>
+      </c>
+      <c r="W80">
+        <v>1.75</v>
       </c>
       <c r="X80">
         <v>0</v>
@@ -5970,7 +6687,7 @@
         <v>0</v>
       </c>
       <c r="Z80">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:26">
@@ -6022,8 +6739,23 @@
       <c r="Q81">
         <v>1</v>
       </c>
+      <c r="R81">
+        <v>0</v>
+      </c>
+      <c r="S81">
+        <v>1.55</v>
+      </c>
+      <c r="T81">
+        <v>4</v>
+      </c>
+      <c r="U81">
+        <v>6.5</v>
+      </c>
       <c r="V81">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="W81">
+        <v>4</v>
       </c>
       <c r="X81">
         <v>0</v>
@@ -6032,7 +6764,7 @@
         <v>0</v>
       </c>
       <c r="Z81">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:26">
@@ -6087,11 +6819,32 @@
       <c r="Q82">
         <v>0</v>
       </c>
+      <c r="R82">
+        <v>1</v>
+      </c>
+      <c r="S82">
+        <v>2.9</v>
+      </c>
+      <c r="T82">
+        <v>3.2</v>
+      </c>
+      <c r="U82">
+        <v>2.45</v>
+      </c>
       <c r="V82">
-        <v>0</v>
+        <v>2.9</v>
+      </c>
+      <c r="W82">
+        <v>2.45</v>
+      </c>
+      <c r="X82">
+        <v>3.2</v>
+      </c>
+      <c r="Y82">
+        <v>1.387610619469027</v>
       </c>
       <c r="Z82">
-        <v>0</v>
+        <v>1.99375</v>
       </c>
     </row>
     <row r="83" spans="1:26">
@@ -6300,11 +7053,32 @@
       <c r="Q85">
         <v>1</v>
       </c>
+      <c r="R85">
+        <v>-1</v>
+      </c>
+      <c r="S85">
+        <v>2.55</v>
+      </c>
+      <c r="T85">
+        <v>3.3</v>
+      </c>
+      <c r="U85">
+        <v>2.7</v>
+      </c>
       <c r="V85">
-        <v>0</v>
+        <v>2.7</v>
+      </c>
+      <c r="W85">
+        <v>2.7</v>
+      </c>
+      <c r="X85">
+        <v>3.3</v>
+      </c>
+      <c r="Y85">
+        <v>1.485</v>
       </c>
       <c r="Z85">
-        <v>0</v>
+        <v>1.881818181818182</v>
       </c>
     </row>
     <row r="86" spans="1:26">
@@ -6433,8 +7207,23 @@
       <c r="Q87">
         <v>0</v>
       </c>
+      <c r="R87">
+        <v>0</v>
+      </c>
+      <c r="S87">
+        <v>1.83</v>
+      </c>
+      <c r="T87">
+        <v>3.6</v>
+      </c>
+      <c r="U87">
+        <v>4.2</v>
+      </c>
       <c r="V87">
-        <v>0</v>
+        <v>3.6</v>
+      </c>
+      <c r="W87">
+        <v>1.83</v>
       </c>
       <c r="X87">
         <v>0</v>
@@ -6443,7 +7232,7 @@
         <v>0</v>
       </c>
       <c r="Z87">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:26">
@@ -6495,8 +7284,23 @@
       <c r="Q88">
         <v>1</v>
       </c>
+      <c r="R88">
+        <v>1</v>
+      </c>
+      <c r="S88">
+        <v>1.25</v>
+      </c>
+      <c r="T88">
+        <v>6</v>
+      </c>
+      <c r="U88">
+        <v>10</v>
+      </c>
       <c r="V88">
-        <v>0</v>
+        <v>1.25</v>
+      </c>
+      <c r="W88">
+        <v>1.25</v>
       </c>
       <c r="X88">
         <v>0</v>
@@ -6505,7 +7309,7 @@
         <v>0</v>
       </c>
       <c r="Z88">
-        <v>0</v>
+        <v>1.041666666666667</v>
       </c>
     </row>
     <row r="89" spans="1:26">
@@ -6634,8 +7438,23 @@
       <c r="Q90">
         <v>0</v>
       </c>
+      <c r="R90">
+        <v>0</v>
+      </c>
+      <c r="S90">
+        <v>1.61</v>
+      </c>
+      <c r="T90">
+        <v>4.2</v>
+      </c>
+      <c r="U90">
+        <v>5.5</v>
+      </c>
       <c r="V90">
-        <v>0</v>
+        <v>4.2</v>
+      </c>
+      <c r="W90">
+        <v>1.61</v>
       </c>
       <c r="X90">
         <v>0</v>
@@ -6644,7 +7463,7 @@
         <v>0</v>
       </c>
       <c r="Z90">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:26">
@@ -6696,8 +7515,23 @@
       <c r="Q91">
         <v>0</v>
       </c>
+      <c r="R91">
+        <v>1</v>
+      </c>
+      <c r="S91">
+        <v>1.28</v>
+      </c>
+      <c r="T91">
+        <v>5.75</v>
+      </c>
+      <c r="U91">
+        <v>9</v>
+      </c>
       <c r="V91">
-        <v>0</v>
+        <v>1.28</v>
+      </c>
+      <c r="W91">
+        <v>5.75</v>
       </c>
       <c r="X91">
         <v>0</v>
@@ -6706,7 +7540,7 @@
         <v>0</v>
       </c>
       <c r="Z91">
-        <v>0</v>
+        <v>1.057391304347826</v>
       </c>
     </row>
     <row r="92" spans="1:26">
@@ -6912,8 +7746,23 @@
       <c r="Q94">
         <v>0</v>
       </c>
+      <c r="R94">
+        <v>1</v>
+      </c>
+      <c r="S94">
+        <v>2.15</v>
+      </c>
+      <c r="T94">
+        <v>3.75</v>
+      </c>
+      <c r="U94">
+        <v>3</v>
+      </c>
       <c r="V94">
-        <v>0</v>
+        <v>2.15</v>
+      </c>
+      <c r="W94">
+        <v>3.75</v>
       </c>
       <c r="X94">
         <v>0</v>
@@ -6922,7 +7771,7 @@
         <v>0</v>
       </c>
       <c r="Z94">
-        <v>0</v>
+        <v>1.576666666666667</v>
       </c>
     </row>
     <row r="95" spans="1:26">
@@ -6974,8 +7823,23 @@
       <c r="Q95">
         <v>1</v>
       </c>
+      <c r="R95">
+        <v>0</v>
+      </c>
+      <c r="S95">
+        <v>1.8</v>
+      </c>
+      <c r="T95">
+        <v>3.5</v>
+      </c>
+      <c r="U95">
+        <v>4.5</v>
+      </c>
       <c r="V95">
-        <v>0</v>
+        <v>3.5</v>
+      </c>
+      <c r="W95">
+        <v>3.5</v>
       </c>
       <c r="X95">
         <v>0</v>
@@ -6984,7 +7848,7 @@
         <v>0</v>
       </c>
       <c r="Z95">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:26">
@@ -7036,8 +7900,23 @@
       <c r="Q96">
         <v>1</v>
       </c>
+      <c r="R96">
+        <v>1</v>
+      </c>
+      <c r="S96">
+        <v>1.4</v>
+      </c>
+      <c r="T96">
+        <v>5</v>
+      </c>
+      <c r="U96">
+        <v>6.5</v>
+      </c>
       <c r="V96">
-        <v>0</v>
+        <v>1.4</v>
+      </c>
+      <c r="W96">
+        <v>1.4</v>
       </c>
       <c r="X96">
         <v>0</v>
@@ -7046,7 +7925,7 @@
         <v>0</v>
       </c>
       <c r="Z96">
-        <v>0</v>
+        <v>1.12</v>
       </c>
     </row>
     <row r="97" spans="1:26">
@@ -7175,8 +8054,23 @@
       <c r="Q98">
         <v>1</v>
       </c>
+      <c r="R98">
+        <v>1</v>
+      </c>
+      <c r="S98">
+        <v>2.1</v>
+      </c>
+      <c r="T98">
+        <v>3.25</v>
+      </c>
+      <c r="U98">
+        <v>3.6</v>
+      </c>
       <c r="V98">
-        <v>0</v>
+        <v>2.1</v>
+      </c>
+      <c r="W98">
+        <v>2.1</v>
       </c>
       <c r="X98">
         <v>0</v>
@@ -7185,7 +8079,7 @@
         <v>0</v>
       </c>
       <c r="Z98">
-        <v>0</v>
+        <v>1.453846153846154</v>
       </c>
     </row>
     <row r="99" spans="1:26">
@@ -7314,8 +8208,23 @@
       <c r="Q100">
         <v>1</v>
       </c>
+      <c r="R100">
+        <v>1</v>
+      </c>
+      <c r="S100">
+        <v>1.53</v>
+      </c>
+      <c r="T100">
+        <v>3.8</v>
+      </c>
+      <c r="U100">
+        <v>6</v>
+      </c>
       <c r="V100">
-        <v>0</v>
+        <v>1.53</v>
+      </c>
+      <c r="W100">
+        <v>1.53</v>
       </c>
       <c r="X100">
         <v>0</v>
@@ -7324,7 +8233,7 @@
         <v>0</v>
       </c>
       <c r="Z100">
-        <v>0</v>
+        <v>1.127368421052632</v>
       </c>
     </row>
     <row r="101" spans="1:26">
@@ -7376,8 +8285,23 @@
       <c r="Q101">
         <v>0</v>
       </c>
+      <c r="R101">
+        <v>0</v>
+      </c>
+      <c r="S101">
+        <v>8</v>
+      </c>
+      <c r="T101">
+        <v>5</v>
+      </c>
+      <c r="U101">
+        <v>1.36</v>
+      </c>
       <c r="V101">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="W101">
+        <v>1.36</v>
       </c>
       <c r="X101">
         <v>0</v>
@@ -7386,7 +8310,7 @@
         <v>0</v>
       </c>
       <c r="Z101">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:26">
@@ -7592,8 +8516,23 @@
       <c r="Q104">
         <v>1</v>
       </c>
+      <c r="R104">
+        <v>1</v>
+      </c>
+      <c r="S104">
+        <v>1.14</v>
+      </c>
+      <c r="T104">
+        <v>8.5</v>
+      </c>
+      <c r="U104">
+        <v>17</v>
+      </c>
       <c r="V104">
-        <v>0</v>
+        <v>1.14</v>
+      </c>
+      <c r="W104">
+        <v>1.14</v>
       </c>
       <c r="X104">
         <v>0</v>
@@ -7602,7 +8541,7 @@
         <v>0</v>
       </c>
       <c r="Z104">
-        <v>0</v>
+        <v>1.005882352941176</v>
       </c>
     </row>
     <row r="105" spans="1:26">
@@ -7657,11 +8596,32 @@
       <c r="Q105">
         <v>0</v>
       </c>
+      <c r="R105">
+        <v>0</v>
+      </c>
+      <c r="S105">
+        <v>4.2</v>
+      </c>
+      <c r="T105">
+        <v>3.5</v>
+      </c>
+      <c r="U105">
+        <v>1.85</v>
+      </c>
       <c r="V105">
-        <v>0</v>
+        <v>3.5</v>
+      </c>
+      <c r="W105">
+        <v>1.85</v>
+      </c>
+      <c r="X105">
+        <v>3.5</v>
+      </c>
+      <c r="Y105">
+        <v>1.210280373831776</v>
       </c>
       <c r="Z105">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:26">
@@ -7713,8 +8673,23 @@
       <c r="Q106">
         <v>0</v>
       </c>
+      <c r="R106">
+        <v>-1</v>
+      </c>
+      <c r="S106">
+        <v>2.25</v>
+      </c>
+      <c r="T106">
+        <v>3.3</v>
+      </c>
+      <c r="U106">
+        <v>3.2</v>
+      </c>
       <c r="V106">
-        <v>0</v>
+        <v>3.2</v>
+      </c>
+      <c r="W106">
+        <v>3.3</v>
       </c>
       <c r="X106">
         <v>0</v>
@@ -7723,7 +8698,7 @@
         <v>0</v>
       </c>
       <c r="Z106">
-        <v>0</v>
+        <v>2.23030303030303</v>
       </c>
     </row>
     <row r="107" spans="1:26">
@@ -7852,8 +8827,23 @@
       <c r="Q108">
         <v>1</v>
       </c>
+      <c r="R108">
+        <v>0</v>
+      </c>
+      <c r="S108">
+        <v>3.3</v>
+      </c>
+      <c r="T108">
+        <v>3.6</v>
+      </c>
+      <c r="U108">
+        <v>2.1</v>
+      </c>
       <c r="V108">
-        <v>0</v>
+        <v>3.6</v>
+      </c>
+      <c r="W108">
+        <v>3.6</v>
       </c>
       <c r="X108">
         <v>0</v>
@@ -7862,7 +8852,7 @@
         <v>0</v>
       </c>
       <c r="Z108">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:26">
@@ -7914,8 +8904,23 @@
       <c r="Q109">
         <v>1</v>
       </c>
+      <c r="R109">
+        <v>0</v>
+      </c>
+      <c r="S109">
+        <v>2.55</v>
+      </c>
+      <c r="T109">
+        <v>3.2</v>
+      </c>
+      <c r="U109">
+        <v>2.9</v>
+      </c>
       <c r="V109">
-        <v>0</v>
+        <v>3.2</v>
+      </c>
+      <c r="W109">
+        <v>3.2</v>
       </c>
       <c r="X109">
         <v>0</v>
@@ -7924,7 +8929,7 @@
         <v>0</v>
       </c>
       <c r="Z109">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:26">
@@ -8053,8 +9058,23 @@
       <c r="Q111">
         <v>0</v>
       </c>
+      <c r="R111">
+        <v>1</v>
+      </c>
+      <c r="S111">
+        <v>2.87</v>
+      </c>
+      <c r="T111">
+        <v>3</v>
+      </c>
+      <c r="U111">
+        <v>2.7</v>
+      </c>
       <c r="V111">
-        <v>0</v>
+        <v>2.87</v>
+      </c>
+      <c r="W111">
+        <v>3</v>
       </c>
       <c r="X111">
         <v>0</v>
@@ -8063,7 +9083,7 @@
         <v>0</v>
       </c>
       <c r="Z111">
-        <v>0</v>
+        <v>1.913333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>